<commit_message>
Added scatter plots of significant factors
</commit_message>
<xml_diff>
--- a/Correlation_data_color_coded.xlsx
+++ b/Correlation_data_color_coded.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Studies\Spring 2023\Independent Study Revival\Github\Agriculture-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8857ADFC-A205-49A4-9E98-804C9331120C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86B207F-87E7-4041-A8A5-8D1B21F05094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42975" yWindow="2670" windowWidth="22440" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Country</t>
   </si>
@@ -98,6 +111,24 @@
   </si>
   <si>
     <t>Romania</t>
+  </si>
+  <si>
+    <t>High positive correlation</t>
+  </si>
+  <si>
+    <t>Low positive correlation</t>
+  </si>
+  <si>
+    <t>Low negative correlation</t>
+  </si>
+  <si>
+    <t>High negative correlation</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
@@ -118,12 +149,36 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,16 +208,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -188,48 +251,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -531,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,23 +1091,172 @@
         <v>-0.03</v>
       </c>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7">
+        <f>AVERAGE(B2:B12)</f>
+        <v>0.77727272727272723</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13:O13" si="0">AVERAGE(C2:C12)</f>
+        <v>0.78181818181818175</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.16</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.1818181818181817E-2</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58454545454545448</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.55272727272727284</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.46272727272727282</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.7272727272727259E-2</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.15777777777777777</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.10818181818181817</v>
+      </c>
+      <c r="N13" s="7">
+        <f t="shared" si="0"/>
+        <v>-7.8181818181818144E-2</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.10399999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7">
+        <f>_xlfn.STDEV.S(B2:B12)</f>
+        <v>0.19688021277370266</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" ref="C14:O14" si="1">_xlfn.STDEV.S(C2:C12)</f>
+        <v>0.20252497040208106</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.25811818998280611</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.24387776371855557</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.35005713819318129</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32296636469959639</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.43717481421259624</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.53267421392612779</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.59773055650670748</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.57977006936658371</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32881521321928592</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.46499071349475751</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.56186863556917255</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.59488934545286098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C16" s="4"/>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="3"/>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C19" s="5"/>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O12">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+      <formula>-0.3</formula>
       <formula>0</formula>
-      <formula>0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>-0.3</formula>
+      <formula>-1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>0.3</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
-      <formula>-0.3</formula>
-      <formula>-1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
-      <formula>-0.3</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
       <formula>0</formula>
+      <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated correlation analysis insights
</commit_message>
<xml_diff>
--- a/Correlation_data_color_coded.xlsx
+++ b/Correlation_data_color_coded.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Studies\Spring 2023\Independent Study Revival\Github\Agriculture-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86B207F-87E7-4041-A8A5-8D1B21F05094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8904FF9A-1951-4528-B713-B9E6C4BBB40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42975" yWindow="2670" windowWidth="22440" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Country</t>
   </si>
@@ -125,10 +125,7 @@
     <t>High negative correlation</t>
   </si>
   <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Standard Deviation</t>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -552,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1096,147 +1093,72 @@
         <v>30</v>
       </c>
       <c r="B13" s="7">
-        <f>AVERAGE(B2:B12)</f>
-        <v>0.77727272727272723</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:O13" si="0">AVERAGE(C2:C12)</f>
-        <v>0.78181818181818175</v>
+        <v>11</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.16</v>
+        <v>3</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>4.1818181818181817E-2</v>
+        <v>2</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>7</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.58454545454545448</v>
+        <v>9</v>
       </c>
       <c r="H13" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.55272727272727284</v>
+        <v>9</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.46272727272727282</v>
+        <v>8</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.7272727272727259E-2</v>
+        <v>8</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
+        <v>3</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.15777777777777777</v>
+        <v>5</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.10818181818181817</v>
+        <v>7</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="0"/>
-        <v>-7.8181818181818144E-2</v>
+        <v>8</v>
       </c>
       <c r="O13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.10399999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="7">
-        <f>_xlfn.STDEV.S(B2:B12)</f>
-        <v>0.19688021277370266</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" ref="C14:O14" si="1">_xlfn.STDEV.S(C2:C12)</f>
-        <v>0.20252497040208106</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.25811818998280611</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.24387776371855557</v>
-      </c>
-      <c r="F14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.35005713819318129</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.32296636469959639</v>
-      </c>
-      <c r="H14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.43717481421259624</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.53267421392612779</v>
-      </c>
-      <c r="J14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59773055650670748</v>
-      </c>
-      <c r="K14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.57977006936658371</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.32881521321928592</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.46499071349475751</v>
-      </c>
-      <c r="N14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.56186863556917255</v>
-      </c>
-      <c r="O14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59488934545286098</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C16" s="4"/>
+      <c r="C16" s="3"/>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="3"/>
+      <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C18" s="2"/>
+      <c r="C18" s="5"/>
       <c r="D18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C19" s="5"/>
-      <c r="D19" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>